<commit_message>
Start implementing test code
</commit_message>
<xml_diff>
--- a/dq/use_case/usecase_definition.xlsx
+++ b/dq/use_case/usecase_definition.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Usecase</t>
   </si>
@@ -159,13 +159,10 @@
     <t>SDMFFP2</t>
   </si>
   <si>
-    <t>Medi</t>
-  </si>
-  <si>
-    <t>Kat</t>
-  </si>
-  <si>
-    <t>Nick</t>
+    <t>UseCase2</t>
+  </si>
+  <si>
+    <t>UseCase3</t>
   </si>
 </sst>
 </file>
@@ -528,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR6"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -707,17 +704,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implementing add_assessment_result_to_matrix and some other minor changes
</commit_message>
<xml_diff>
--- a/dq/use_case/usecase_definition.xlsx
+++ b/dq/use_case/usecase_definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bdr-dq-main\bdr-dq\dq\use_case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DQAF\pythonProject1\dq\use_case\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="177">
   <si>
     <t>Data quality assertion</t>
   </si>
@@ -547,19 +547,16 @@
     <t>If the datum link reference in the 'geo:hasGeometry' field does not correspond to any of the specified types (AGD84, GDA2020, GDA94, WGS84), label the record as 'None'. This label indicates that the datum used does not match the predefined types, suggesting either a different standard is in use or the datum type is unspecified.</t>
   </si>
   <si>
-    <t>Baseline-SDMFFP1</t>
-  </si>
-  <si>
-    <t>Baseline-SDMFFP2</t>
-  </si>
-  <si>
-    <t>Baseline-SDMFFP3</t>
+    <t>SDMFFP1</t>
+  </si>
+  <si>
+    <t>SDMFFP2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -926,19 +923,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -948,21 +945,15 @@
       <c r="C1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -970,9 +961,8 @@
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -980,327 +970,296 @@
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1315,18 +1274,18 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.53125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.06640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.06640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="54.9296875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="40.19921875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="4"/>
+    <col min="1" max="1" width="47.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="55" style="4" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1346,7 +1305,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1366,7 +1325,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1386,7 +1345,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1406,7 +1365,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -1426,7 +1385,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1446,7 +1405,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1466,7 +1425,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1486,7 +1445,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1506,7 +1465,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -1526,7 +1485,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -1546,7 +1505,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -1566,7 +1525,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -1586,7 +1545,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -1606,7 +1565,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -1626,7 +1585,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
@@ -1646,7 +1605,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
@@ -1666,7 +1625,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="171" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1686,7 +1645,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -1706,7 +1665,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -1726,7 +1685,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -1746,7 +1705,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
@@ -1766,7 +1725,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -1786,7 +1745,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
@@ -1806,7 +1765,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
@@ -1826,7 +1785,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>25</v>
       </c>
@@ -1846,7 +1805,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
@@ -1866,7 +1825,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
@@ -1886,7 +1845,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
@@ -1906,7 +1865,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
@@ -1926,7 +1885,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
@@ -1946,7 +1905,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
@@ -1966,7 +1925,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
@@ -1986,7 +1945,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
@@ -2006,7 +1965,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
@@ -2026,7 +1985,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
@@ -2046,7 +2005,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>36</v>
       </c>
@@ -2066,7 +2025,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>37</v>
       </c>
@@ -2086,7 +2045,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>38</v>
       </c>
@@ -2106,7 +2065,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>39</v>
       </c>
@@ -2126,7 +2085,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
@@ -2146,7 +2105,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>41</v>
       </c>
@@ -2166,7 +2125,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>42</v>
       </c>
@@ -2186,7 +2145,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>43</v>
       </c>

</xml_diff>